<commit_message>
Implemented the rest of the experiments
</commit_message>
<xml_diff>
--- a/plots/experiment4_conditional.xlsx
+++ b/plots/experiment4_conditional.xlsx
@@ -555,25 +555,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0008</v>
+        <v>0.0012</v>
       </c>
       <c r="D4" t="n">
-        <v>608.298</v>
+        <v>508.5162</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.9465</v>
+        <v>16.7674</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4993</v>
+        <v>0.55</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0341</v>
+        <v>0.07530000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4428</v>
+        <v>0.5002</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0037</v>
+        <v>0.0477</v>
       </c>
     </row>
     <row r="5">
@@ -584,25 +584,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0011</v>
+        <v>0.0008</v>
       </c>
       <c r="D5" t="n">
-        <v>453.081</v>
+        <v>478.4193</v>
       </c>
       <c r="E5" t="n">
-        <v>4.9968</v>
+        <v>3.9519</v>
       </c>
       <c r="F5" t="n">
-        <v>0.311</v>
+        <v>0.5511</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0301</v>
+        <v>0.007900000000000001</v>
       </c>
       <c r="H5" t="n">
-        <v>0.505</v>
+        <v>0.4654</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0489</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -613,25 +613,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.015</v>
+        <v>0.0146</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.8298</v>
+        <v>0.6108</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.9563</v>
+        <v>-25.9108</v>
       </c>
       <c r="F6" t="n">
-        <v>0.476</v>
+        <v>0.3197</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.0022</v>
       </c>
       <c r="H6" t="n">
-        <v>0.493</v>
+        <v>0.4817</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0047</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="7">
@@ -642,25 +642,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.007900000000000001</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.4684</v>
+        <v>3.1412</v>
       </c>
       <c r="E7" t="n">
-        <v>5.4774</v>
+        <v>7.408</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6567</v>
+        <v>0.5508999999999999</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0005</v>
+        <v>0.0004</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4581</v>
+        <v>0.3747</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0062</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="8">
@@ -675,25 +675,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0172</v>
+        <v>0.0168</v>
       </c>
       <c r="D8" t="n">
-        <v>160.0399</v>
+        <v>148.9547</v>
       </c>
       <c r="E8" t="n">
-        <v>1.3594</v>
+        <v>2.2989</v>
       </c>
       <c r="F8" t="n">
-        <v>86061.3374</v>
+        <v>86021.67389999999</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>31501.7197</v>
+        <v>68590.1407</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0005</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -704,25 +704,25 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0116</v>
+        <v>0.0115</v>
       </c>
       <c r="D9" t="n">
-        <v>160.5368</v>
+        <v>166.5822</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6738</v>
+        <v>0.1339</v>
       </c>
       <c r="F9" t="n">
-        <v>65410.1669</v>
+        <v>114613.889</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0158</v>
+        <v>0.004</v>
       </c>
       <c r="H9" t="n">
-        <v>31222.2153</v>
+        <v>113051.0417</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0041</v>
+        <v>0.0013</v>
       </c>
     </row>
     <row r="10">
@@ -733,25 +733,25 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0044</v>
+        <v>0.0045</v>
       </c>
       <c r="D10" t="n">
-        <v>50.852</v>
+        <v>53.0471</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.1006</v>
+        <v>-0.1748</v>
       </c>
       <c r="F10" t="n">
-        <v>2.4215</v>
+        <v>2.089</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>2.2172</v>
+        <v>2.1426</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0183</v>
+        <v>0.0239</v>
       </c>
     </row>
     <row r="11">
@@ -762,25 +762,25 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0432</v>
+        <v>0.0437</v>
       </c>
       <c r="D11" t="n">
-        <v>603.0006</v>
+        <v>601.4115</v>
       </c>
       <c r="E11" t="n">
-        <v>2.8524</v>
+        <v>1.3951</v>
       </c>
       <c r="F11" t="n">
-        <v>5364.9943</v>
+        <v>6283.6503</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0059</v>
+        <v>0.0031</v>
       </c>
       <c r="H11" t="n">
-        <v>4447.4237</v>
+        <v>4444.9265</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0091</v>
+        <v>0.0031</v>
       </c>
     </row>
     <row r="12">
@@ -795,25 +795,25 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0246</v>
+        <v>0.0245</v>
       </c>
       <c r="D12" t="n">
-        <v>69.7167</v>
+        <v>29.4255</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.0527</v>
+        <v>2.6811</v>
       </c>
       <c r="F12" t="n">
-        <v>1.7057</v>
+        <v>1.594</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1266</v>
+        <v>0.2259</v>
       </c>
       <c r="H12" t="n">
-        <v>1.6957</v>
+        <v>1.515</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0964</v>
+        <v>0.06270000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -824,25 +824,25 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0089</v>
+        <v>0.0091</v>
       </c>
       <c r="D13" t="n">
-        <v>36.7268</v>
+        <v>8.411199999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>5.4678</v>
+        <v>0.5188</v>
       </c>
       <c r="F13" t="n">
-        <v>0.847</v>
+        <v>0.7977</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1769</v>
+        <v>0.2831</v>
       </c>
       <c r="H13" t="n">
-        <v>0.7575</v>
+        <v>0.7688</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0287</v>
+        <v>0.1621</v>
       </c>
     </row>
     <row r="14">
@@ -856,22 +856,22 @@
         <v>0.0051</v>
       </c>
       <c r="D14" t="n">
-        <v>102.3795</v>
+        <v>4154.2697</v>
       </c>
       <c r="E14" t="n">
-        <v>-274.3767</v>
+        <v>13.0684</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5478</v>
+        <v>0.2559</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3599</v>
+        <v>0.2025</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4325</v>
+        <v>0.2794</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1559</v>
+        <v>0.2574</v>
       </c>
     </row>
     <row r="15">
@@ -882,25 +882,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.07190000000000001</v>
+        <v>0.0718</v>
       </c>
       <c r="D15" t="n">
-        <v>175.2175</v>
+        <v>1486.0761</v>
       </c>
       <c r="E15" t="n">
-        <v>16.7996</v>
+        <v>16.1801</v>
       </c>
       <c r="F15" t="n">
-        <v>0.982</v>
+        <v>0.9927</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4726</v>
+        <v>0.4948</v>
       </c>
       <c r="H15" t="n">
-        <v>0.9578</v>
+        <v>0.9388</v>
       </c>
       <c r="I15" t="n">
-        <v>0.5295</v>
+        <v>0.6129</v>
       </c>
     </row>
     <row r="16">
@@ -915,25 +915,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.0387</v>
+        <v>0.0391</v>
       </c>
       <c r="D16" t="n">
-        <v>74.357</v>
+        <v>68.9068</v>
       </c>
       <c r="E16" t="n">
-        <v>-5.471</v>
+        <v>0.2887</v>
       </c>
       <c r="F16" t="n">
-        <v>2.7687</v>
+        <v>2.5567</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1026</v>
+        <v>0.1512</v>
       </c>
       <c r="H16" t="n">
-        <v>2.4434</v>
+        <v>2.7311</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1372</v>
+        <v>0.0882</v>
       </c>
     </row>
     <row r="17">
@@ -944,25 +944,25 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.005</v>
+        <v>0.0049</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1485</v>
+        <v>-0.8939</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.1253</v>
+        <v>3.778</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5155</v>
+        <v>0.5053</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3063</v>
+        <v>0.118</v>
       </c>
       <c r="H17" t="n">
-        <v>0.5054999999999999</v>
+        <v>0.4864</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2558</v>
+        <v>0.2481</v>
       </c>
     </row>
     <row r="18">
@@ -973,25 +973,25 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0011</v>
+        <v>0.0009</v>
       </c>
       <c r="D18" t="n">
-        <v>10.0218</v>
+        <v>7.6487</v>
       </c>
       <c r="E18" t="n">
-        <v>3.1573</v>
+        <v>1.7074</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5054</v>
+        <v>0.482</v>
       </c>
       <c r="G18" t="n">
-        <v>0.047</v>
+        <v>0.0366</v>
       </c>
       <c r="H18" t="n">
-        <v>0.4832</v>
+        <v>0.4962</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0218</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1005,22 +1005,22 @@
         <v>0.0058</v>
       </c>
       <c r="D19" t="n">
-        <v>5.765</v>
+        <v>3.0299</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2399</v>
+        <v>1.2246</v>
       </c>
       <c r="F19" t="n">
-        <v>2.6303</v>
+        <v>2.6395</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0131</v>
+        <v>0.0182</v>
       </c>
       <c r="H19" t="n">
-        <v>2.6065</v>
+        <v>2.513</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0124</v>
+        <v>0.009299999999999999</v>
       </c>
     </row>
     <row r="20">
@@ -1035,25 +1035,25 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.0266</v>
+        <v>0.0546</v>
       </c>
       <c r="D20" t="n">
-        <v>2.2761</v>
+        <v>0.4447</v>
       </c>
       <c r="E20" t="n">
-        <v>1.6275</v>
+        <v>5.7306</v>
       </c>
       <c r="F20" t="n">
-        <v>2.9893</v>
+        <v>3.0314</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0761</v>
+        <v>0.1319</v>
       </c>
       <c r="H20" t="n">
-        <v>2.8513</v>
+        <v>2.7474</v>
       </c>
       <c r="I20" t="n">
-        <v>0.1119</v>
+        <v>0.1357</v>
       </c>
     </row>
     <row r="21">
@@ -1064,25 +1064,25 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.9043</v>
+        <v>0.8934</v>
       </c>
       <c r="D21" t="n">
-        <v>503.0673</v>
+        <v>507.1132</v>
       </c>
       <c r="E21" t="n">
-        <v>-10.1636</v>
+        <v>-5.181</v>
       </c>
       <c r="F21" t="n">
-        <v>93151.2626</v>
+        <v>87205.6191</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2197</v>
+        <v>0.1832</v>
       </c>
       <c r="H21" t="n">
-        <v>74352.681</v>
+        <v>71983.50599999999</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0413</v>
+        <v>0.2457</v>
       </c>
     </row>
     <row r="22">
@@ -1093,25 +1093,25 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.0139</v>
+        <v>0.0303</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1581</v>
+        <v>-2.3016</v>
       </c>
       <c r="E22" t="n">
-        <v>8.419</v>
+        <v>-7.5272</v>
       </c>
       <c r="F22" t="n">
-        <v>2.8897</v>
+        <v>3.2474</v>
       </c>
       <c r="G22" t="n">
-        <v>0.147</v>
+        <v>0.0516</v>
       </c>
       <c r="H22" t="n">
-        <v>2.7062</v>
+        <v>2.7512</v>
       </c>
       <c r="I22" t="n">
-        <v>0.1063</v>
+        <v>0.0679</v>
       </c>
     </row>
     <row r="23">
@@ -1122,25 +1122,25 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.6412</v>
+        <v>0.6404</v>
       </c>
       <c r="D23" t="n">
-        <v>459.3539</v>
+        <v>458.5277</v>
       </c>
       <c r="E23" t="n">
-        <v>8.861499999999999</v>
+        <v>4.3641</v>
       </c>
       <c r="F23" t="n">
-        <v>100771.0238</v>
+        <v>92676.80409999999</v>
       </c>
       <c r="G23" t="n">
-        <v>0.008699999999999999</v>
+        <v>0.0868</v>
       </c>
       <c r="H23" t="n">
-        <v>76045.86870000001</v>
+        <v>76425.2227</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1461</v>
+        <v>0.1492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>